<commit_message>
1. calculated the consumption ce and total wealth ce 2. used income_test data
</commit_message>
<xml_diff>
--- a/results/ce.xlsx
+++ b/results/ce.xlsx
@@ -405,10 +405,10 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>15646.25251349266</v>
+        <v>15470.62290791229</v>
       </c>
       <c r="C2">
-        <v>468054.4120987031</v>
+        <v>847722.6056723457</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -416,10 +416,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>22148.4273940486</v>
+        <v>23739.24350645736</v>
       </c>
       <c r="C3">
-        <v>633465.6104425318</v>
+        <v>1300806.921723364</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -427,10 +427,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>37868.70679675952</v>
+        <v>38346.253017191</v>
       </c>
       <c r="C4">
-        <v>991013.7372928722</v>
+        <v>2101207.282925812</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use vectorized method instead of a for-loop to calculate the ce data
</commit_message>
<xml_diff>
--- a/results/ce.xlsx
+++ b/results/ce.xlsx
@@ -405,10 +405,10 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>15470.62290791229</v>
+        <v>15755.97779219088</v>
       </c>
       <c r="C2">
-        <v>847722.6056723457</v>
+        <v>863358.8077491384</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -416,10 +416,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>23739.24350645736</v>
+        <v>23775.99974660412</v>
       </c>
       <c r="C3">
-        <v>1300806.921723364</v>
+        <v>1302821.003241439</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -427,10 +427,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>38346.253017191</v>
+        <v>38780.97304745853</v>
       </c>
       <c r="C4">
-        <v>2101207.282925812</v>
+        <v>2125028.043019956</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use the new survival probability
</commit_message>
<xml_diff>
--- a/results/ce.xlsx
+++ b/results/ce.xlsx
@@ -405,10 +405,10 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>15755.97779219088</v>
+        <v>15052.56464127515</v>
       </c>
       <c r="C2">
-        <v>863358.8077491384</v>
+        <v>824814.8374961047</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -416,10 +416,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>23775.99974660412</v>
+        <v>22348.25969763185</v>
       </c>
       <c r="C3">
-        <v>1302821.003241439</v>
+        <v>1224587.080681118</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -427,10 +427,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>38780.97304745853</v>
+        <v>34777.10901857738</v>
       </c>
       <c r="C4">
-        <v>2125028.043019956</v>
+        <v>1905633.771210448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit before adding a new branch
</commit_message>
<xml_diff>
--- a/results/ce.xlsx
+++ b/results/ce.xlsx
@@ -405,10 +405,10 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>15052.56464127515</v>
+        <v>13364.84712035547</v>
       </c>
       <c r="C2">
-        <v>824814.8374961047</v>
+        <v>570778.8208882479</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -416,10 +416,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>22348.25969763185</v>
+        <v>21256.78294175362</v>
       </c>
       <c r="C3">
-        <v>1224587.080681118</v>
+        <v>907823.4411594858</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -427,10 +427,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>34777.10901857738</v>
+        <v>27475.93170723113</v>
       </c>
       <c r="C4">
-        <v>1905633.771210448</v>
+        <v>1173427.556741277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>